<commit_message>
NC data is omitted; agg level 1 is roughly complete
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/TEST-mapping.xlsx
+++ b/input/extension/user-defined-energy/TEST-mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16560" yWindow="460" windowWidth="12240" windowHeight="17440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16560" yWindow="460" windowWidth="12240" windowHeight="17440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CEDS_sector" sheetId="1" r:id="rId1"/>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>